<commit_message>
ui for search results
</commit_message>
<xml_diff>
--- a/goTripcyContent/resources/excel/data.xlsx
+++ b/goTripcyContent/resources/excel/data.xlsx
@@ -770,19 +770,19 @@
     <t>2</t>
   </si>
   <si>
-    <t>standard,deluxe,luxury</t>
-  </si>
-  <si>
-    <t>34999,39999,44999</t>
-  </si>
-  <si>
-    <t>25999,31999,38999</t>
-  </si>
-  <si>
-    <t>31999,38999,42999</t>
-  </si>
-  <si>
     <t>Image</t>
+  </si>
+  <si>
+    <t>standard;;;deluxe;;;luxury</t>
+  </si>
+  <si>
+    <t>34999;;;39999;;;44999</t>
+  </si>
+  <si>
+    <t>25999;;;31999;;;38999</t>
+  </si>
+  <si>
+    <t>31999;;;38999;;;42999</t>
   </si>
 </sst>
 </file>
@@ -2516,8 +2516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2605,7 +2605,7 @@
         <v>246</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="18.75" customHeight="1">
@@ -2650,13 +2650,13 @@
         <v>226</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>227</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
@@ -2730,13 +2730,13 @@
         <v>229</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>227</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
@@ -2810,13 +2810,13 @@
         <v>231</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="P6" s="4" t="s">
         <v>227</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>

</xml_diff>